<commit_message>
Format values in the output json
</commit_message>
<xml_diff>
--- a/database/paths.xlsx
+++ b/database/paths.xlsx
@@ -12,48 +12,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">massif </t>
+  </si>
+  <si>
     <t>code</t>
   </si>
   <si>
-    <t>name</t>
+    <t>description</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>reverseTime</t>
   </si>
   <si>
     <t>nickname</t>
   </si>
   <si>
-    <t xml:space="preserve">massif </t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>sign</t>
-  </si>
-  <si>
     <t>countyCode</t>
   </si>
   <si>
-    <t>points</t>
-  </si>
-  <si>
-    <t>tracks</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>reverseTime</t>
-  </si>
-  <si>
     <t>countyName</t>
   </si>
   <si>
-    <t>alitude</t>
+    <t>altitude</t>
   </si>
   <si>
     <t>publicTransport</t>
@@ -62,12 +59,12 @@
     <t xml:space="preserve">car </t>
   </si>
   <si>
+    <t>CBARN</t>
+  </si>
+  <si>
     <t>Barnova</t>
   </si>
   <si>
-    <t>CBARN</t>
-  </si>
-  <si>
     <t>blue dot</t>
   </si>
   <si>
@@ -92,15 +89,21 @@
     <t>[2, 3]</t>
   </si>
   <si>
+    <t>red triangle</t>
+  </si>
+  <si>
+    <t>[3, 1]</t>
+  </si>
+  <si>
+    <t>red stripe</t>
+  </si>
+  <si>
+    <t>[14, 1]</t>
+  </si>
+  <si>
     <t>Iasi</t>
   </si>
   <si>
-    <t>red triangle</t>
-  </si>
-  <si>
-    <t>[3, 1]</t>
-  </si>
-  <si>
     <t>PSCHIT</t>
   </si>
   <si>
@@ -110,10 +113,7 @@
     <t>Rezervatie floristica</t>
   </si>
   <si>
-    <t>red stripe</t>
-  </si>
-  <si>
-    <t>[14, 1]</t>
+    <t>[1, 3, 5, 9]</t>
   </si>
   <si>
     <t>PCETATE</t>
@@ -122,15 +122,12 @@
     <t>Poiana cu Cetate</t>
   </si>
   <si>
+    <t>red cross</t>
+  </si>
+  <si>
     <t>Biserica lui Cujba</t>
   </si>
   <si>
-    <t>[1, 3, 5, 9]</t>
-  </si>
-  <si>
-    <t>red cross</t>
-  </si>
-  <si>
     <t>[7, 8]</t>
   </si>
   <si>
@@ -152,10 +149,10 @@
     <t>RADARB</t>
   </si>
   <si>
+    <t>[14, 1, 4, 6, 11]</t>
+  </si>
+  <si>
     <t>Observatoru Meteo Barnova</t>
-  </si>
-  <si>
-    <t>[14, 1, 4, 6, 11]</t>
   </si>
   <si>
     <t>Radar Barnova</t>
@@ -171,10 +168,10 @@
 drum forestier</t>
   </si>
   <si>
+    <t>[9, 4]</t>
+  </si>
+  <si>
     <t>CANVAMA</t>
-  </si>
-  <si>
-    <t>[9, 4]</t>
   </si>
   <si>
     <t>Cantonul Palanca</t>
@@ -546,34 +543,34 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -581,25 +578,25 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I4" s="3">
         <v>200.0</v>
@@ -616,22 +613,22 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I5" s="3">
         <v>220.0</v>
@@ -648,17 +645,17 @@
         <v>35</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I6" s="3">
         <v>190.0</v>
@@ -669,22 +666,22 @@
         <v>4.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I7" s="3">
         <v>230.0</v>
@@ -701,16 +698,16 @@
         <v>52</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -718,19 +715,19 @@
         <v>6.0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
@@ -738,19 +735,19 @@
         <v>7.0</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J10" s="3">
         <v>1.0</v>
@@ -761,19 +758,19 @@
         <v>8.0</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -781,19 +778,19 @@
         <v>9.0</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J12" s="3">
         <v>1.0</v>
@@ -807,19 +804,19 @@
         <v>10.0</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
@@ -827,22 +824,22 @@
         <v>11.0</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="E14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="3">
@@ -854,19 +851,19 @@
         <v>12.0</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
@@ -874,19 +871,19 @@
         <v>13.0</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="E16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -894,30 +891,25 @@
         <v>14.0</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="E17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J17" s="3">
         <v>1.0</v>
       </c>
       <c r="K17" s="3">
         <v>1.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +930,6 @@
     <col customWidth="1" min="1" max="1" width="7.29"/>
     <col customWidth="1" min="5" max="5" width="16.29"/>
     <col customWidth="1" min="6" max="6" width="18.0"/>
-    <col customWidth="1" min="7" max="7" width="16.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -946,28 +937,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -978,15 +966,15 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45.0</v>
       </c>
       <c r="H2" s="3">
-        <v>45.0</v>
-      </c>
-      <c r="I2" s="3">
         <v>45.0</v>
       </c>
     </row>
@@ -995,12 +983,12 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3" s="3">
         <v>45.0</v>
       </c>
     </row>
@@ -1009,12 +997,12 @@
         <v>3.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="3">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3">
         <v>60.0</v>
       </c>
     </row>
@@ -1023,15 +1011,15 @@
         <v>4.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45.0</v>
       </c>
       <c r="H5" s="3">
-        <v>45.0</v>
-      </c>
-      <c r="I5" s="3">
         <v>30.0</v>
       </c>
     </row>
@@ -1040,12 +1028,12 @@
         <v>5.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="3">
+        <v>33</v>
+      </c>
+      <c r="G6" s="3">
         <v>180.0</v>
       </c>
     </row>
@@ -1054,12 +1042,12 @@
         <v>6.0</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="3">
         <v>240.0</v>
       </c>
     </row>
@@ -1068,12 +1056,12 @@
         <v>7.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="3">
+        <v>39</v>
+      </c>
+      <c r="G8" s="3">
         <v>180.0</v>
       </c>
     </row>
@@ -1082,15 +1070,15 @@
         <v>8.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="G9" s="3">
+        <v>60.0</v>
       </c>
       <c r="H9" s="3">
-        <v>60.0</v>
-      </c>
-      <c r="I9" s="3">
         <v>50.0</v>
       </c>
     </row>
@@ -1099,15 +1087,15 @@
         <v>9.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="G10" s="3">
+        <v>40.0</v>
       </c>
       <c r="H10" s="3">
-        <v>40.0</v>
-      </c>
-      <c r="I10" s="3">
         <v>60.0</v>
       </c>
     </row>
@@ -1116,12 +1104,12 @@
         <v>10.0</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11" s="3">
         <v>30.0</v>
       </c>
     </row>
@@ -1130,12 +1118,12 @@
         <v>11.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="3">
+        <v>45</v>
+      </c>
+      <c r="G12" s="3">
         <v>300.0</v>
       </c>
     </row>
@@ -1144,12 +1132,12 @@
         <v>12.0</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="4">
         <v>180.0</v>
       </c>
     </row>
@@ -1158,28 +1146,13 @@
         <v>13.0</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="G14" s="3">
         <v>180.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3">
-        <v>16.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>